<commit_message>
Added ability to make groups
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Coward\Desktop\python project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Coward\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC16BB96-B1BC-42C9-AFE5-4F0349E2541F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB9BC71-E291-4B9C-A3CE-B9965D4D1221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="12">
   <si>
     <t>E</t>
   </si>
@@ -50,6 +50,18 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
   </si>
 </sst>
 </file>
@@ -59,10 +71,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -168,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -176,12 +194,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -466,47 +482,47 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="M1" t="s">
         <v>2</v>
@@ -516,38 +532,38 @@
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>0</v>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="M2" t="s">
         <v>3</v>
@@ -557,38 +573,38 @@
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>0</v>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" t="s">
+        <v>9</v>
       </c>
       <c r="M3" t="s">
         <v>1</v>
@@ -598,38 +614,38 @@
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>0</v>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" t="s">
+        <v>9</v>
       </c>
       <c r="M4" t="s">
         <v>4</v>
@@ -639,38 +655,38 @@
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>0</v>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" t="s">
+        <v>10</v>
       </c>
       <c r="M5" t="s">
         <v>0</v>
@@ -680,38 +696,38 @@
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>0</v>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" t="s">
+        <v>10</v>
       </c>
       <c r="M6" t="s">
         <v>5</v>
@@ -721,86 +737,86 @@
       <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>0</v>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" t="s">
+        <v>11</v>
       </c>
       <c r="M7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>0</v>
+      <c r="A8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" t="s">
+        <v>11</v>
       </c>
       <c r="M8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="4">
         <v>1</v>
       </c>
       <c r="B9">
@@ -809,7 +825,7 @@
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="4">
         <v>4</v>
       </c>
       <c r="E9">
@@ -818,7 +834,7 @@
       <c r="F9">
         <v>6</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="4">
         <v>7</v>
       </c>
       <c r="H9">
@@ -827,7 +843,7 @@
       <c r="I9">
         <v>9</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="4">
         <v>10</v>
       </c>
       <c r="K9">
@@ -838,6 +854,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -847,7 +864,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M8"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,17 +895,7 @@
       <c r="A2" s="4">
         <v>1.111</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="6"/>
+      <c r="L2" s="5"/>
       <c r="M2" t="s">
         <v>3</v>
       </c>
@@ -897,17 +904,7 @@
       <c r="A3" s="4">
         <v>0.123</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="6"/>
+      <c r="L3" s="5"/>
       <c r="M3" t="s">
         <v>1</v>
       </c>
@@ -916,17 +913,7 @@
       <c r="A4" s="4">
         <v>1.4E-2</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="6"/>
+      <c r="L4" s="5"/>
       <c r="M4" t="s">
         <v>4</v>
       </c>
@@ -935,17 +922,7 @@
       <c r="A5" s="4">
         <v>1.5200000000000001E-3</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="6"/>
+      <c r="L5" s="5"/>
       <c r="M5" t="s">
         <v>0</v>
       </c>
@@ -954,17 +931,7 @@
       <c r="A6" s="4">
         <v>1.6899999999999999E-4</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="6"/>
+      <c r="L6" s="5"/>
       <c r="M6" t="s">
         <v>5</v>
       </c>
@@ -973,42 +940,32 @@
       <c r="A7" s="4">
         <v>1.88E-5</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="6"/>
+      <c r="L7" s="5"/>
       <c r="M7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>2.0899999999999999E-6</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="9"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="8"/>
       <c r="M8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="4">
         <v>1</v>
       </c>
       <c r="B9">
@@ -1017,7 +974,7 @@
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="4">
         <v>4</v>
       </c>
       <c r="E9">
@@ -1026,7 +983,7 @@
       <c r="F9">
         <v>6</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="4">
         <v>7</v>
       </c>
       <c r="H9">
@@ -1035,7 +992,7 @@
       <c r="I9">
         <v>9</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="4">
         <v>10</v>
       </c>
       <c r="K9">

</xml_diff>